<commit_message>
implement sample weight 2
</commit_message>
<xml_diff>
--- a/misc/curve_info_to_QC.xlsx
+++ b/misc/curve_info_to_QC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian Liu\Documents\Project\SPEGCS ML Challenge\project-gcs-datathon2021\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E84CF6-BC84-486F-A512-79FE7AF3268A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0AEBE3-EE2A-4B15-8B0E-38BEA562A888}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="3810" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="254">
   <si>
     <t>WellNo</t>
   </si>
@@ -773,6 +773,15 @@
   </si>
   <si>
     <t>start here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DT2, DT1, DT4S, DT4P, DTST, </t>
+  </si>
+  <si>
+    <t>DTSM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTCO  </t>
   </si>
 </sst>
 </file>
@@ -1619,8 +1628,8 @@
   <dimension ref="A1:E236"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <pane ySplit="2" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N116" sqref="N116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2439,7 +2448,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>94</v>
       </c>
@@ -2447,7 +2456,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>95</v>
       </c>
@@ -2455,7 +2464,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>96</v>
       </c>
@@ -2463,7 +2472,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>97</v>
       </c>
@@ -2471,7 +2480,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>98</v>
       </c>
@@ -2479,7 +2488,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>99</v>
       </c>
@@ -2487,7 +2496,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>100</v>
       </c>
@@ -2495,7 +2504,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>101</v>
       </c>
@@ -2503,7 +2512,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>102</v>
       </c>
@@ -2511,7 +2520,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>103</v>
       </c>
@@ -2519,7 +2528,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>104</v>
       </c>
@@ -2527,15 +2536,18 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>105</v>
       </c>
       <c r="B108" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>106</v>
       </c>
@@ -2543,7 +2555,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>107</v>
       </c>
@@ -2551,7 +2563,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>108</v>
       </c>
@@ -2559,7 +2571,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>109</v>
       </c>
@@ -2567,7 +2579,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>110</v>
       </c>
@@ -2575,7 +2587,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>111</v>
       </c>
@@ -2583,7 +2595,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>112</v>
       </c>
@@ -2591,7 +2603,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>113</v>
       </c>
@@ -2599,7 +2611,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>114</v>
       </c>
@@ -2607,15 +2619,18 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>115</v>
       </c>
       <c r="B118" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>116</v>
       </c>
@@ -2623,7 +2638,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>117</v>
       </c>
@@ -2631,7 +2646,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>118</v>
       </c>
@@ -2639,7 +2654,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>119</v>
       </c>
@@ -2647,7 +2662,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>120</v>
       </c>
@@ -2655,7 +2670,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>121</v>
       </c>
@@ -2663,7 +2678,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>122</v>
       </c>
@@ -2671,7 +2686,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>123</v>
       </c>
@@ -2679,7 +2694,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>124</v>
       </c>
@@ -2687,7 +2702,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>125</v>
       </c>
@@ -2823,7 +2838,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>142</v>
       </c>
@@ -2831,7 +2846,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>143</v>
       </c>
@@ -2839,7 +2854,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>144</v>
       </c>
@@ -2847,7 +2862,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>145</v>
       </c>
@@ -2855,7 +2870,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>146</v>
       </c>
@@ -2863,7 +2878,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>147</v>
       </c>
@@ -2871,7 +2886,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>148</v>
       </c>
@@ -2879,7 +2894,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>149</v>
       </c>
@@ -2887,7 +2902,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>150</v>
       </c>
@@ -2895,7 +2910,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>151</v>
       </c>
@@ -2903,7 +2918,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>152</v>
       </c>
@@ -2911,7 +2926,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>153</v>
       </c>
@@ -2919,15 +2934,18 @@
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>154</v>
       </c>
       <c r="B157" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C157" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>155</v>
       </c>
@@ -2935,7 +2953,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>156</v>
       </c>
@@ -2943,7 +2961,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>157</v>
       </c>
@@ -2951,7 +2969,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>158</v>
       </c>
@@ -2959,7 +2977,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>159</v>
       </c>
@@ -2967,7 +2985,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>160</v>
       </c>
@@ -2975,7 +2993,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>161</v>
       </c>
@@ -2983,7 +3001,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>162</v>
       </c>
@@ -2991,15 +3009,18 @@
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>163</v>
       </c>
       <c r="B166" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C166" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>164</v>
       </c>
@@ -3007,7 +3028,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>165</v>
       </c>
@@ -3015,7 +3036,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>166</v>
       </c>
@@ -3023,7 +3044,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>167</v>
       </c>
@@ -3031,7 +3052,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>168</v>
       </c>
@@ -3039,7 +3060,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>169</v>
       </c>
@@ -3047,7 +3068,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>170</v>
       </c>
@@ -3055,7 +3076,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>171</v>
       </c>
@@ -3063,7 +3084,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>172</v>
       </c>
@@ -3071,7 +3092,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>173</v>
       </c>
@@ -3338,15 +3359,18 @@
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>206</v>
       </c>
       <c r="B209" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C209" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>207</v>
       </c>
@@ -3354,7 +3378,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>208</v>
       </c>
@@ -3362,7 +3386,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>209</v>
       </c>
@@ -3370,7 +3394,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>210</v>
       </c>
@@ -3378,7 +3402,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>211</v>
       </c>
@@ -3386,7 +3410,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>212</v>
       </c>
@@ -3394,7 +3418,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>213</v>
       </c>
@@ -3402,7 +3426,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>214</v>
       </c>
@@ -3410,7 +3434,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>215</v>
       </c>
@@ -3418,7 +3442,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>216</v>
       </c>
@@ -3426,7 +3450,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>217</v>
       </c>
@@ -3434,7 +3458,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>218</v>
       </c>
@@ -3442,7 +3466,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>219</v>
       </c>
@@ -3450,7 +3474,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>220</v>
       </c>
@@ -3458,7 +3482,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>221</v>
       </c>

</xml_diff>

<commit_message>
added leaderboard 1 data
</commit_message>
<xml_diff>
--- a/misc/curve_info_to_QC.xlsx
+++ b/misc/curve_info_to_QC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian Liu\Documents\Project\SPEGCS ML Challenge\project-gcs-datathon2021\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DE342C-CE73-4599-B68C-8C73EEBB11AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E160C90D-E534-4062-9673-BB0635C37BA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="3810" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="curve_info_to_QC" sheetId="1" r:id="rId1"/>
@@ -787,13 +787,13 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>too deep, depth : 16-22k ft</t>
-  </si>
-  <si>
     <t>too shallow, 2-3k ft</t>
   </si>
   <si>
     <t>DT, DTM</t>
+  </si>
+  <si>
+    <t>too deep, depth : 16-22k ft, probably lateral, looking at the GR range</t>
   </si>
 </sst>
 </file>
@@ -1637,8 +1637,8 @@
   <dimension ref="A1:G235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2114,7 +2114,7 @@
         <v>52</v>
       </c>
       <c r="C52" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -2595,7 +2595,7 @@
         <v>1</v>
       </c>
       <c r="G111" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -2892,7 +2892,7 @@
         <v>1</v>
       </c>
       <c r="G147" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -3264,7 +3264,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>191</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>192</v>
       </c>
@@ -3280,15 +3280,18 @@
         <v>194</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>193</v>
       </c>
       <c r="B195" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E195">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>194</v>
       </c>
@@ -3296,7 +3299,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>195</v>
       </c>
@@ -3304,7 +3307,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>196</v>
       </c>
@@ -3312,7 +3315,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>197</v>
       </c>
@@ -3320,7 +3323,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>198</v>
       </c>
@@ -3328,7 +3331,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>199</v>
       </c>
@@ -3336,7 +3339,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>200</v>
       </c>
@@ -3344,7 +3347,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>201</v>
       </c>
@@ -3352,7 +3355,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>202</v>
       </c>
@@ -3360,7 +3363,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>203</v>
       </c>
@@ -3368,7 +3371,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>204</v>
       </c>
@@ -3376,7 +3379,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>205</v>
       </c>
@@ -3384,7 +3387,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>206</v>
       </c>

</xml_diff>